<commit_message>
-Pass input file for AFM volume scan through command line.
</commit_message>
<xml_diff>
--- a/volumetric_scan_AFM_sync.xlsx
+++ b/volumetric_scan_AFM_sync.xlsx
@@ -540,7 +540,7 @@
   <dimension ref="A1:CG30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="AY32" sqref="AY32"/>
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,6 +552,13 @@
       <c r="A1" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
     </row>
     <row r="4" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">

</xml_diff>